<commit_message>
pyinstaller missing binary fixed
</commit_message>
<xml_diff>
--- a/2_output/outputFile.xlsx
+++ b/2_output/outputFile.xlsx
@@ -41,7 +41,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -54,12 +54,12 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -68,7 +68,7 @@
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -475,7 +475,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>C:\Users\DT0083\Desktop\Python Learning\ezVideoThumbnails\1_input\SBM_MV_1080×1080_220117_iP13pro_gp_nts_YDN.mp4</t>
+          <t>C:\Users\DT0083\Desktop\Python-Learning\ezVideoThumbnails\1_input\SBM_MV_1080×1080_220117_iP13pro_gp_nts_YDN.mp4</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -486,13 +486,21 @@
       <c r="C2" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="inlineStr"/>
-      <c r="E2" s="2" t="inlineStr"/>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>C:\Users\DT0083\Desktop\Python-Learning\ezVideoThumbnails\2_output\SBM_MV_1080×1080_220117_iP13pro_gp_nts_YDN.jpg</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>SBM_MV_1080×1080_220117_iP13pro_gp_nts_YDN.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>C:\Users\DT0083\Desktop\Python Learning\ezVideoThumbnails\1_input\SBM_MV_1080×1080_220117_iP13_bl_olaf_YDN.mp4</t>
+          <t>C:\Users\DT0083\Desktop\Python-Learning\ezVideoThumbnails\1_input\SBM_MV_1080×1080_220117_iP13_bl_olaf_YDN.mp4</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -503,13 +511,21 @@
       <c r="C3" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="inlineStr"/>
-      <c r="E3" s="2" t="inlineStr"/>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>C:\Users\DT0083\Desktop\Python-Learning\ezVideoThumbnails\2_output\SBM_MV_1080×1080_220117_iP13_bl_olaf_YDN.jpg</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>SBM_MV_1080×1080_220117_iP13_bl_olaf_YDN.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>C:\Users\DT0083\Desktop\Python Learning\ezVideoThumbnails\1_input\SBM_MV_1280×720_220117_iP13pro_sibl_nts_YDN.mp4</t>
+          <t>C:\Users\DT0083\Desktop\Python-Learning\ezVideoThumbnails\1_input\SBM_MV_1280×720_220117_iP13pro_sibl_nts_YDN.mp4</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -520,13 +536,21 @@
       <c r="C4" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="D4" s="2" t="inlineStr"/>
-      <c r="E4" s="2" t="inlineStr"/>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>C:\Users\DT0083\Desktop\Python-Learning\ezVideoThumbnails\2_output\SBM_MV_1280×720_220117_iP13pro_sibl_nts_YDN.jpg</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>SBM_MV_1280×720_220117_iP13pro_sibl_nts_YDN.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>C:\Users\DT0083\Desktop\Python Learning\ezVideoThumbnails\1_input\SBM_MV_1280×720_220117_iP13_mdn_olaf_YDN.mp4</t>
+          <t>C:\Users\DT0083\Desktop\Python-Learning\ezVideoThumbnails\1_input\SBM_MV_1280×720_220117_iP13_mdn_olaf_YDN.mp4</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -537,8 +561,16 @@
       <c r="C5" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="D5" s="2" t="inlineStr"/>
-      <c r="E5" s="2" t="inlineStr"/>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>C:\Users\DT0083\Desktop\Python-Learning\ezVideoThumbnails\2_output\SBM_MV_1280×720_220117_iP13_mdn_olaf_YDN.jpg</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>SBM_MV_1280×720_220117_iP13_mdn_olaf_YDN.jpg</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>